<commit_message>
Minor change: 'dataset_neuroscience1' to 'dataset_neuroscience_1'.
</commit_message>
<xml_diff>
--- a/data/dataset_neuroscience_vo.xlsx
+++ b/data/dataset_neuroscience_vo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MDASILVA\MDASILVA\ESEO\INTERSHIP\BDA\BDA_Project\BDAJupiterNotebook\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7F0C02-F859-4080-9D95-4354BEECE09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F73610D-47F9-4ED5-8704-8F50900A11EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{C829A673-F44C-49DE-8E9A-B2FC9AA259F4}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="745">
   <si>
     <t>animal</t>
   </si>
@@ -2256,9 +2256,6 @@
   </si>
   <si>
     <t>Unknown</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -2654,7 +2651,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -2897,19 +2894,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -2983,7 +2967,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -2996,32 +2980,31 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
@@ -4114,8 +4097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{665CECC1-8FBB-4BDB-A4F2-9DF141040273}">
   <dimension ref="A1:BO317"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E306" sqref="E306"/>
+    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
+      <selection activeCell="C317" sqref="C317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4136,393 +4119,393 @@
       <c r="C1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="P1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="R1" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="S1" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="T1" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="U1" s="22" t="s">
+      <c r="U1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="V1" s="22" t="s">
+      <c r="V1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="W1" s="22" t="s">
+      <c r="W1" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="X1" s="22" t="s">
+      <c r="X1" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="Y1" s="22" t="s">
+      <c r="Y1" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="Z1" s="22" t="s">
+      <c r="Z1" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="AA1" s="23" t="s">
+      <c r="AA1" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="AB1" s="24" t="s">
+      <c r="AB1" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="AC1" s="25" t="s">
+      <c r="AC1" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="AD1" s="25" t="s">
+      <c r="AD1" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="AE1" s="25" t="s">
+      <c r="AE1" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="AF1" s="25" t="s">
+      <c r="AF1" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="AG1" s="25" t="s">
+      <c r="AG1" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="AH1" s="25" t="s">
+      <c r="AH1" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="AI1" s="26" t="s">
+      <c r="AI1" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="AJ1" s="27" t="s">
+      <c r="AJ1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="AK1" s="28" t="s">
+      <c r="AK1" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="AL1" s="28" t="s">
+      <c r="AL1" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="AM1" s="28" t="s">
+      <c r="AM1" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="AN1" s="28" t="s">
+      <c r="AN1" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="AO1" s="28" t="s">
+      <c r="AO1" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="AP1" s="28" t="s">
+      <c r="AP1" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="AQ1" s="29" t="s">
+      <c r="AQ1" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="AR1" s="30" t="s">
+      <c r="AR1" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="AS1" s="31" t="s">
+      <c r="AS1" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="AT1" s="31" t="s">
+      <c r="AT1" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="AU1" s="31" t="s">
+      <c r="AU1" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="AV1" s="31" t="s">
+      <c r="AV1" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="AW1" s="31" t="s">
+      <c r="AW1" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="AX1" s="31" t="s">
+      <c r="AX1" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="AY1" s="32" t="s">
+      <c r="AY1" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="AZ1" s="33" t="s">
+      <c r="AZ1" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="BA1" s="34" t="s">
+      <c r="BA1" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="BB1" s="34" t="s">
+      <c r="BB1" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="BC1" s="34" t="s">
+      <c r="BC1" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="BD1" s="34" t="s">
+      <c r="BD1" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="BE1" s="34" t="s">
+      <c r="BE1" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="BF1" s="34" t="s">
+      <c r="BF1" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="BG1" s="35" t="s">
+      <c r="BG1" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="BH1" s="36" t="s">
+      <c r="BH1" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="BI1" s="37" t="s">
+      <c r="BI1" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="BJ1" s="37" t="s">
+      <c r="BJ1" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="BK1" s="37" t="s">
+      <c r="BK1" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="BL1" s="37" t="s">
+      <c r="BL1" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="BM1" s="37" t="s">
+      <c r="BM1" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="BN1" s="37" t="s">
+      <c r="BN1" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="BO1" s="38" t="s">
+      <c r="BO1" s="37" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.3">
-      <c r="A2" s="39"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42" t="s">
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="I2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="42" t="s">
+      <c r="J2" s="41" t="s">
         <v>744</v>
       </c>
-      <c r="K2" s="42" t="s">
+      <c r="K2" s="41" t="s">
         <v>744</v>
       </c>
-      <c r="L2" s="42" t="s">
+      <c r="L2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="42" t="s">
+      <c r="M2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="42" t="s">
+      <c r="N2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="42" t="s">
+      <c r="O2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="42" t="s">
+      <c r="P2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="42" t="s">
+      <c r="Q2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="42" t="s">
+      <c r="R2" s="41" t="s">
         <v>744</v>
       </c>
-      <c r="S2" s="42" t="s">
+      <c r="S2" s="41" t="s">
         <v>744</v>
       </c>
-      <c r="T2" s="42" t="s">
+      <c r="T2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="U2" s="42" t="s">
+      <c r="U2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="V2" s="42" t="s">
+      <c r="V2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="W2" s="42" t="s">
+      <c r="W2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="X2" s="42" t="s">
+      <c r="X2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="42" t="s">
+      <c r="Y2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="Z2" s="42" t="s">
+      <c r="Z2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="AA2" s="42" t="s">
+      <c r="AA2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="AB2" s="42" t="s">
+      <c r="AB2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="AC2" s="42" t="s">
+      <c r="AC2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="AD2" s="42" t="s">
+      <c r="AD2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="AE2" s="42" t="s">
+      <c r="AE2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="AF2" s="42" t="s">
+      <c r="AF2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="AG2" s="42" t="s">
+      <c r="AG2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="AH2" s="42" t="s">
+      <c r="AH2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="AI2" s="42" t="s">
+      <c r="AI2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="AJ2" s="42" t="s">
+      <c r="AJ2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="AK2" s="42" t="s">
+      <c r="AK2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="AL2" s="42" t="s">
+      <c r="AL2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="AM2" s="42" t="s">
+      <c r="AM2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="AN2" s="42" t="s">
+      <c r="AN2" s="41" t="s">
         <v>744</v>
       </c>
-      <c r="AO2" s="42" t="s">
+      <c r="AO2" s="41" t="s">
         <v>744</v>
       </c>
-      <c r="AP2" s="42" t="s">
+      <c r="AP2" s="41" t="s">
         <v>744</v>
       </c>
-      <c r="AQ2" s="42" t="s">
+      <c r="AQ2" s="41" t="s">
         <v>744</v>
       </c>
-      <c r="AR2" s="42" t="s">
+      <c r="AR2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="AS2" s="42" t="s">
+      <c r="AS2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="AT2" s="42" t="s">
+      <c r="AT2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="AU2" s="42" t="s">
+      <c r="AU2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="AV2" s="42" t="s">
+      <c r="AV2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="AW2" s="42" t="s">
+      <c r="AW2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="AX2" s="42" t="s">
+      <c r="AX2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="AY2" s="42" t="s">
+      <c r="AY2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="AZ2" s="42" t="s">
+      <c r="AZ2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="BA2" s="42" t="s">
+      <c r="BA2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="BB2" s="42" t="s">
+      <c r="BB2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="BC2" s="42" t="s">
+      <c r="BC2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="BD2" s="42" t="s">
+      <c r="BD2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="BE2" s="42" t="s">
+      <c r="BE2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="BF2" s="42" t="s">
+      <c r="BF2" s="41" t="s">
         <v>744</v>
       </c>
-      <c r="BG2" s="42" t="s">
+      <c r="BG2" s="41" t="s">
         <v>744</v>
       </c>
-      <c r="BH2" s="42" t="s">
+      <c r="BH2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="BI2" s="42" t="s">
+      <c r="BI2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="BJ2" s="42" t="s">
+      <c r="BJ2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="BK2" s="42" t="s">
+      <c r="BK2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="BL2" s="42" t="s">
+      <c r="BL2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="BM2" s="42" t="s">
+      <c r="BM2" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="BN2" s="42" t="s">
+      <c r="BN2" s="41" t="s">
         <v>744</v>
       </c>
-      <c r="BO2" s="42" t="s">
+      <c r="BO2" s="41" t="s">
         <v>744</v>
       </c>
     </row>
@@ -4539,22 +4522,22 @@
       <c r="D3" s="1">
         <v>9574</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="15">
         <v>7781</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="15">
         <v>17598</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="15">
         <v>4425</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="15">
         <v>7428</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="15">
         <v>8302</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="15">
         <v>4288</v>
       </c>
       <c r="K3" s="2">
@@ -4563,22 +4546,22 @@
       <c r="L3" s="1">
         <v>2527</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M3" s="15">
         <v>3366</v>
       </c>
-      <c r="N3" s="16">
+      <c r="N3" s="15">
         <v>2431</v>
       </c>
-      <c r="O3" s="16">
+      <c r="O3" s="15">
         <v>15881</v>
       </c>
-      <c r="P3" s="16">
+      <c r="P3" s="15">
         <v>17294</v>
       </c>
-      <c r="Q3" s="16">
+      <c r="Q3" s="15">
         <v>10002</v>
       </c>
-      <c r="R3" s="16">
+      <c r="R3" s="15">
         <v>10655</v>
       </c>
       <c r="S3" s="2">
@@ -4587,22 +4570,22 @@
       <c r="T3" s="1">
         <v>4297</v>
       </c>
-      <c r="U3" s="16">
+      <c r="U3" s="15">
         <v>2320</v>
       </c>
-      <c r="V3" s="16">
+      <c r="V3" s="15">
         <v>1873</v>
       </c>
-      <c r="W3" s="16">
+      <c r="W3" s="15">
         <v>3262</v>
       </c>
-      <c r="X3" s="16">
+      <c r="X3" s="15">
         <v>2331</v>
       </c>
-      <c r="Y3" s="16">
+      <c r="Y3" s="15">
         <v>1737</v>
       </c>
-      <c r="Z3" s="16">
+      <c r="Z3" s="15">
         <v>6635</v>
       </c>
       <c r="AA3" s="2">
@@ -4611,22 +4594,22 @@
       <c r="AB3" s="1">
         <v>775</v>
       </c>
-      <c r="AC3" s="16">
+      <c r="AC3" s="15">
         <v>1302</v>
       </c>
-      <c r="AD3" s="16">
+      <c r="AD3" s="15">
         <v>833</v>
       </c>
-      <c r="AE3" s="16">
+      <c r="AE3" s="15">
         <v>1647</v>
       </c>
-      <c r="AF3" s="16">
+      <c r="AF3" s="15">
         <v>1570</v>
       </c>
-      <c r="AG3" s="16">
+      <c r="AG3" s="15">
         <v>1614</v>
       </c>
-      <c r="AH3" s="16">
+      <c r="AH3" s="15">
         <v>896</v>
       </c>
       <c r="AI3" s="2">
@@ -4635,22 +4618,22 @@
       <c r="AJ3" s="1">
         <v>2831</v>
       </c>
-      <c r="AK3" s="16">
+      <c r="AK3" s="15">
         <v>9015</v>
       </c>
-      <c r="AL3" s="16">
+      <c r="AL3" s="15">
         <v>1917</v>
       </c>
-      <c r="AM3" s="16">
+      <c r="AM3" s="15">
         <v>9439</v>
       </c>
-      <c r="AN3" s="16">
+      <c r="AN3" s="15">
         <v>7207</v>
       </c>
-      <c r="AO3" s="16">
+      <c r="AO3" s="15">
         <v>11913</v>
       </c>
-      <c r="AP3" s="16">
+      <c r="AP3" s="15">
         <v>5499</v>
       </c>
       <c r="AQ3" s="2">
@@ -4659,22 +4642,22 @@
       <c r="AR3" s="1">
         <v>14101</v>
       </c>
-      <c r="AS3" s="16">
+      <c r="AS3" s="15">
         <v>14080</v>
       </c>
-      <c r="AT3" s="16">
+      <c r="AT3" s="15">
         <v>13021</v>
       </c>
-      <c r="AU3" s="16">
+      <c r="AU3" s="15">
         <v>14608</v>
       </c>
-      <c r="AV3" s="16">
+      <c r="AV3" s="15">
         <v>13623</v>
       </c>
-      <c r="AW3" s="16">
+      <c r="AW3" s="15">
         <v>14286</v>
       </c>
-      <c r="AX3" s="16">
+      <c r="AX3" s="15">
         <v>13326</v>
       </c>
       <c r="AY3" s="2">
@@ -4683,22 +4666,22 @@
       <c r="AZ3" s="1">
         <v>2980</v>
       </c>
-      <c r="BA3" s="16">
+      <c r="BA3" s="15">
         <v>9268</v>
       </c>
-      <c r="BB3" s="16">
+      <c r="BB3" s="15">
         <v>1655</v>
       </c>
-      <c r="BC3" s="16">
+      <c r="BC3" s="15">
         <v>6935</v>
       </c>
-      <c r="BD3" s="16">
+      <c r="BD3" s="15">
         <v>3343</v>
       </c>
-      <c r="BE3" s="16">
+      <c r="BE3" s="15">
         <v>12453</v>
       </c>
-      <c r="BF3" s="16">
+      <c r="BF3" s="15">
         <v>3367</v>
       </c>
       <c r="BG3" s="2">
@@ -4707,22 +4690,22 @@
       <c r="BH3" s="1">
         <v>7404</v>
       </c>
-      <c r="BI3" s="16">
+      <c r="BI3" s="15">
         <v>4925</v>
       </c>
-      <c r="BJ3" s="16">
+      <c r="BJ3" s="15">
         <v>12521</v>
       </c>
-      <c r="BK3" s="16">
+      <c r="BK3" s="15">
         <v>10363</v>
       </c>
-      <c r="BL3" s="16">
+      <c r="BL3" s="15">
         <v>4562</v>
       </c>
-      <c r="BM3" s="16">
+      <c r="BM3" s="15">
         <v>14383</v>
       </c>
-      <c r="BN3" s="16">
+      <c r="BN3" s="15">
         <v>789</v>
       </c>
       <c r="BO3" s="2">
@@ -68275,28 +68258,28 @@
       <c r="B317" s="6" t="s">
         <v>743</v>
       </c>
-      <c r="C317" s="12" t="s">
-        <v>745</v>
+      <c r="C317" s="11" t="s">
+        <v>709</v>
       </c>
       <c r="D317" s="5">
         <v>76</v>
       </c>
-      <c r="E317" s="17">
+      <c r="E317" s="16">
         <v>67</v>
       </c>
-      <c r="F317" s="17">
+      <c r="F317" s="16">
         <v>163</v>
       </c>
-      <c r="G317" s="17">
+      <c r="G317" s="16">
         <v>111</v>
       </c>
-      <c r="H317" s="17">
+      <c r="H317" s="16">
         <v>66</v>
       </c>
-      <c r="I317" s="17">
+      <c r="I317" s="16">
         <v>284</v>
       </c>
-      <c r="J317" s="17">
+      <c r="J317" s="16">
         <v>0</v>
       </c>
       <c r="K317" s="6">
@@ -68305,22 +68288,22 @@
       <c r="L317" s="5">
         <v>1</v>
       </c>
-      <c r="M317" s="17">
+      <c r="M317" s="16">
         <v>239</v>
       </c>
-      <c r="N317" s="17">
+      <c r="N317" s="16">
         <v>31</v>
       </c>
-      <c r="O317" s="17">
+      <c r="O317" s="16">
         <v>3</v>
       </c>
-      <c r="P317" s="17">
+      <c r="P317" s="16">
         <v>232</v>
       </c>
-      <c r="Q317" s="17">
+      <c r="Q317" s="16">
         <v>52</v>
       </c>
-      <c r="R317" s="17">
+      <c r="R317" s="16">
         <v>13</v>
       </c>
       <c r="S317" s="6">
@@ -68329,22 +68312,22 @@
       <c r="T317" s="5">
         <v>12</v>
       </c>
-      <c r="U317" s="17">
+      <c r="U317" s="16">
         <v>19</v>
       </c>
-      <c r="V317" s="17">
+      <c r="V317" s="16">
         <v>38</v>
       </c>
-      <c r="W317" s="17">
+      <c r="W317" s="16">
         <v>28</v>
       </c>
-      <c r="X317" s="17">
+      <c r="X317" s="16">
         <v>198</v>
       </c>
-      <c r="Y317" s="17">
+      <c r="Y317" s="16">
         <v>18</v>
       </c>
-      <c r="Z317" s="17">
+      <c r="Z317" s="16">
         <v>8</v>
       </c>
       <c r="AA317" s="6">
@@ -68353,22 +68336,22 @@
       <c r="AB317" s="5">
         <v>6</v>
       </c>
-      <c r="AC317" s="17">
+      <c r="AC317" s="16">
         <v>1</v>
       </c>
-      <c r="AD317" s="17">
+      <c r="AD317" s="16">
         <v>57</v>
       </c>
-      <c r="AE317" s="17">
+      <c r="AE317" s="16">
         <v>2</v>
       </c>
-      <c r="AF317" s="17">
+      <c r="AF317" s="16">
         <v>11</v>
       </c>
-      <c r="AG317" s="17">
+      <c r="AG317" s="16">
         <v>16</v>
       </c>
-      <c r="AH317" s="17">
+      <c r="AH317" s="16">
         <v>41</v>
       </c>
       <c r="AI317" s="6">
@@ -68377,22 +68360,22 @@
       <c r="AJ317" s="5">
         <v>29</v>
       </c>
-      <c r="AK317" s="17">
+      <c r="AK317" s="16">
         <v>29</v>
       </c>
-      <c r="AL317" s="17">
+      <c r="AL317" s="16">
         <v>124</v>
       </c>
-      <c r="AM317" s="17">
+      <c r="AM317" s="16">
         <v>24</v>
       </c>
-      <c r="AN317" s="17">
+      <c r="AN317" s="16">
         <v>35</v>
       </c>
-      <c r="AO317" s="17">
+      <c r="AO317" s="16">
         <v>113</v>
       </c>
-      <c r="AP317" s="17">
+      <c r="AP317" s="16">
         <v>50</v>
       </c>
       <c r="AQ317" s="6">
@@ -68401,22 +68384,22 @@
       <c r="AR317" s="5">
         <v>30</v>
       </c>
-      <c r="AS317" s="17">
+      <c r="AS317" s="16">
         <v>23</v>
       </c>
-      <c r="AT317" s="17">
+      <c r="AT317" s="16">
         <v>17</v>
       </c>
-      <c r="AU317" s="17">
+      <c r="AU317" s="16">
         <v>22</v>
       </c>
-      <c r="AV317" s="17">
+      <c r="AV317" s="16">
         <v>35</v>
       </c>
-      <c r="AW317" s="17">
+      <c r="AW317" s="16">
         <v>25</v>
       </c>
-      <c r="AX317" s="17">
+      <c r="AX317" s="16">
         <v>14</v>
       </c>
       <c r="AY317" s="6">
@@ -68425,22 +68408,22 @@
       <c r="AZ317" s="5">
         <v>15</v>
       </c>
-      <c r="BA317" s="17">
+      <c r="BA317" s="16">
         <v>4</v>
       </c>
-      <c r="BB317" s="17">
+      <c r="BB317" s="16">
         <v>7</v>
       </c>
-      <c r="BC317" s="17">
+      <c r="BC317" s="16">
         <v>14</v>
       </c>
-      <c r="BD317" s="17">
+      <c r="BD317" s="16">
         <v>64</v>
       </c>
-      <c r="BE317" s="17">
+      <c r="BE317" s="16">
         <v>11</v>
       </c>
-      <c r="BF317" s="17">
+      <c r="BF317" s="16">
         <v>16</v>
       </c>
       <c r="BG317" s="6">
@@ -68449,22 +68432,22 @@
       <c r="BH317" s="5">
         <v>43</v>
       </c>
-      <c r="BI317" s="17">
+      <c r="BI317" s="16">
         <v>2</v>
       </c>
-      <c r="BJ317" s="17">
+      <c r="BJ317" s="16">
         <v>34</v>
       </c>
-      <c r="BK317" s="17">
+      <c r="BK317" s="16">
         <v>27</v>
       </c>
-      <c r="BL317" s="17">
+      <c r="BL317" s="16">
         <v>3</v>
       </c>
-      <c r="BM317" s="17">
+      <c r="BM317" s="16">
         <v>3</v>
       </c>
-      <c r="BN317" s="17">
+      <c r="BN317" s="16">
         <v>0</v>
       </c>
       <c r="BO317" s="6">

</xml_diff>

<commit_message>
I recreated the Jupiter Notebook with nice vision. I'll code the model after.
</commit_message>
<xml_diff>
--- a/data/dataset_neuroscience_vo.xlsx
+++ b/data/dataset_neuroscience_vo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MDASILVA\MDASILVA\ESEO\INTERSHIP\BDA\BDA_Project\BDAJupiterNotebook\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B6C9C4-B366-42BC-849E-7B82CDF90211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A674795-82FB-41DB-90B4-0EE6A90B380C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C829A673-F44C-49DE-8E9A-B2FC9AA259F4}"/>
   </bookViews>
@@ -3297,10 +3297,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{665CECC1-8FBB-4BDB-A4F2-9DF141040273}">
-  <dimension ref="A1:BO323"/>
+  <dimension ref="A1:BO317"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AM321" sqref="AM321"/>
+    <sheetView tabSelected="1" topLeftCell="A317" workbookViewId="0">
+      <selection activeCell="Q328" sqref="Q328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -67656,270 +67656,6 @@
         <v>707</v>
       </c>
     </row>
-    <row r="321" spans="4:67" x14ac:dyDescent="0.3">
-      <c r="D321">
-        <f>SUM(D2:D316)</f>
-        <v>2874169</v>
-      </c>
-      <c r="E321">
-        <f t="shared" ref="E321:BO321" si="0">SUM(E2:E316)</f>
-        <v>2741911</v>
-      </c>
-      <c r="F321">
-        <f t="shared" si="0"/>
-        <v>6084926</v>
-      </c>
-      <c r="G321">
-        <f t="shared" si="0"/>
-        <v>2172441</v>
-      </c>
-      <c r="H321">
-        <f t="shared" si="0"/>
-        <v>2213387</v>
-      </c>
-      <c r="I321">
-        <f t="shared" si="0"/>
-        <v>3073534</v>
-      </c>
-      <c r="J321">
-        <f t="shared" si="0"/>
-        <v>3023897</v>
-      </c>
-      <c r="K321">
-        <f t="shared" si="0"/>
-        <v>2393271</v>
-      </c>
-      <c r="L321">
-        <f t="shared" si="0"/>
-        <v>1540624</v>
-      </c>
-      <c r="M321">
-        <f t="shared" si="0"/>
-        <v>2028787</v>
-      </c>
-      <c r="N321">
-        <f t="shared" si="0"/>
-        <v>1904801</v>
-      </c>
-      <c r="O321">
-        <f t="shared" si="0"/>
-        <v>2710060</v>
-      </c>
-      <c r="P321">
-        <f t="shared" si="0"/>
-        <v>5213341</v>
-      </c>
-      <c r="Q321">
-        <f t="shared" si="0"/>
-        <v>2439566</v>
-      </c>
-      <c r="R321">
-        <f t="shared" si="0"/>
-        <v>2969437</v>
-      </c>
-      <c r="S321">
-        <f t="shared" si="0"/>
-        <v>4878214</v>
-      </c>
-      <c r="T321">
-        <f t="shared" si="0"/>
-        <v>1532878</v>
-      </c>
-      <c r="U321">
-        <f t="shared" si="0"/>
-        <v>2040636</v>
-      </c>
-      <c r="V321">
-        <f t="shared" si="0"/>
-        <v>2414929</v>
-      </c>
-      <c r="W321">
-        <f t="shared" si="0"/>
-        <v>2538250</v>
-      </c>
-      <c r="X321">
-        <f t="shared" si="0"/>
-        <v>2479113</v>
-      </c>
-      <c r="Y321">
-        <f t="shared" si="0"/>
-        <v>2394598</v>
-      </c>
-      <c r="Z321">
-        <f t="shared" si="0"/>
-        <v>1650509</v>
-      </c>
-      <c r="AA321">
-        <f t="shared" si="0"/>
-        <v>1562409</v>
-      </c>
-      <c r="AB321">
-        <f t="shared" si="0"/>
-        <v>878021</v>
-      </c>
-      <c r="AC321">
-        <f t="shared" si="0"/>
-        <v>1326870</v>
-      </c>
-      <c r="AD321">
-        <f t="shared" si="0"/>
-        <v>1151260</v>
-      </c>
-      <c r="AE321">
-        <f t="shared" si="0"/>
-        <v>1254341</v>
-      </c>
-      <c r="AF321">
-        <f t="shared" si="0"/>
-        <v>1167137</v>
-      </c>
-      <c r="AG321">
-        <f t="shared" si="0"/>
-        <v>1462502</v>
-      </c>
-      <c r="AH321">
-        <f t="shared" si="0"/>
-        <v>1555244</v>
-      </c>
-      <c r="AI321">
-        <f t="shared" si="0"/>
-        <v>1031251</v>
-      </c>
-      <c r="AJ321">
-        <f t="shared" si="0"/>
-        <v>2813047</v>
-      </c>
-      <c r="AK321">
-        <f t="shared" si="0"/>
-        <v>2996137</v>
-      </c>
-      <c r="AL321">
-        <f t="shared" si="0"/>
-        <v>2750500</v>
-      </c>
-      <c r="AM321">
-        <f t="shared" si="0"/>
-        <v>6174431</v>
-      </c>
-      <c r="AN321">
-        <f t="shared" si="0"/>
-        <v>2802245</v>
-      </c>
-      <c r="AO321">
-        <f t="shared" si="0"/>
-        <v>3985839</v>
-      </c>
-      <c r="AP321">
-        <f t="shared" si="0"/>
-        <v>2804512</v>
-      </c>
-      <c r="AQ321">
-        <f t="shared" si="0"/>
-        <v>5141505</v>
-      </c>
-      <c r="AR321">
-        <f t="shared" si="0"/>
-        <v>4962783</v>
-      </c>
-      <c r="AS321">
-        <f t="shared" si="0"/>
-        <v>4802318</v>
-      </c>
-      <c r="AT321">
-        <f t="shared" si="0"/>
-        <v>3654292</v>
-      </c>
-      <c r="AU321">
-        <f t="shared" si="0"/>
-        <v>4707371</v>
-      </c>
-      <c r="AV321">
-        <f t="shared" si="0"/>
-        <v>4150196</v>
-      </c>
-      <c r="AW321">
-        <f t="shared" si="0"/>
-        <v>4712711</v>
-      </c>
-      <c r="AX321">
-        <f t="shared" si="0"/>
-        <v>4743384</v>
-      </c>
-      <c r="AY321">
-        <f t="shared" si="0"/>
-        <v>5019285</v>
-      </c>
-      <c r="AZ321">
-        <f t="shared" si="0"/>
-        <v>1273778</v>
-      </c>
-      <c r="BA321">
-        <f t="shared" si="0"/>
-        <v>2326276</v>
-      </c>
-      <c r="BB321">
-        <f t="shared" si="0"/>
-        <v>1557597</v>
-      </c>
-      <c r="BC321">
-        <f t="shared" si="0"/>
-        <v>3267826</v>
-      </c>
-      <c r="BD321">
-        <f t="shared" si="0"/>
-        <v>2070772</v>
-      </c>
-      <c r="BE321">
-        <f t="shared" si="0"/>
-        <v>2618733</v>
-      </c>
-      <c r="BF321">
-        <f t="shared" si="0"/>
-        <v>1727876</v>
-      </c>
-      <c r="BG321">
-        <f t="shared" si="0"/>
-        <v>2008088</v>
-      </c>
-      <c r="BH321">
-        <f t="shared" si="0"/>
-        <v>3433408</v>
-      </c>
-      <c r="BI321">
-        <f t="shared" si="0"/>
-        <v>2408396</v>
-      </c>
-      <c r="BJ321">
-        <f t="shared" si="0"/>
-        <v>2498773</v>
-      </c>
-      <c r="BK321">
-        <f t="shared" si="0"/>
-        <v>916741</v>
-      </c>
-      <c r="BL321">
-        <f t="shared" si="0"/>
-        <v>2420846</v>
-      </c>
-      <c r="BM321">
-        <f t="shared" si="0"/>
-        <v>1841269</v>
-      </c>
-      <c r="BN321">
-        <f t="shared" si="0"/>
-        <v>1139141</v>
-      </c>
-      <c r="BO321">
-        <f t="shared" si="0"/>
-        <v>3856055</v>
-      </c>
-    </row>
-    <row r="323" spans="4:67" x14ac:dyDescent="0.3">
-      <c r="D323">
-        <f>MAX(D321:BO321)</f>
-        <v>6174431</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>